<commit_message>
added inflacion without collapses
</commit_message>
<xml_diff>
--- a/poverty_measurement/output/precios_implicitos.xlsx
+++ b/poverty_measurement/output/precios_implicitos.xlsx
@@ -300,7 +300,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
@@ -308,7 +308,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>60.2205810546875</v>
+        <v>60.441165924072266</v>
       </c>
     </row>
     <row r="21">
@@ -324,7 +324,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
@@ -380,7 +380,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>